<commit_message>
Chapter 7: update on reading Excel files. Typo fixes.
</commit_message>
<xml_diff>
--- a/data/countries_europe.xlsx
+++ b/data/countries_europe.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\ELTE\Oktatás\IntroProg\Notebooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Repos\Lecture\elte_teralg\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{21CD165E-B629-4E5C-B2E7-4C319D411333}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B003B3F-21FF-40B6-BEA1-6AFDE0A08819}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="countries" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="93">
   <si>
     <t>Country</t>
   </si>
@@ -188,9 +188,6 @@
   </si>
   <si>
     <t>Luxembourg</t>
-  </si>
-  <si>
-    <t>luxembourg</t>
   </si>
   <si>
     <t>Macedonia</t>
@@ -307,7 +304,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1160,19 +1157,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -1563,7 +1562,7 @@
         <v>0.03</v>
       </c>
       <c r="E23" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1588,7 +1587,7 @@
         <v>55</v>
       </c>
       <c r="B25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C25">
         <v>2586</v>
@@ -1602,10 +1601,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" t="s">
         <v>57</v>
-      </c>
-      <c r="B26" t="s">
-        <v>58</v>
       </c>
       <c r="C26">
         <v>25713</v>
@@ -1619,10 +1618,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" t="s">
         <v>59</v>
-      </c>
-      <c r="B27" t="s">
-        <v>60</v>
       </c>
       <c r="C27">
         <v>93036</v>
@@ -1636,10 +1635,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" t="s">
         <v>61</v>
-      </c>
-      <c r="B28" t="s">
-        <v>62</v>
       </c>
       <c r="C28">
         <v>316</v>
@@ -1653,10 +1652,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" t="s">
         <v>63</v>
-      </c>
-      <c r="B29" t="s">
-        <v>64</v>
       </c>
       <c r="C29">
         <v>33700</v>
@@ -1665,15 +1664,15 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="E29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C30">
         <v>2</v>
@@ -1687,10 +1686,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" t="s">
         <v>67</v>
-      </c>
-      <c r="B31" t="s">
-        <v>68</v>
       </c>
       <c r="C31">
         <v>13812</v>
@@ -1704,10 +1703,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" t="s">
         <v>69</v>
-      </c>
-      <c r="B32" t="s">
-        <v>70</v>
       </c>
       <c r="C32">
         <v>357042</v>
@@ -1721,10 +1720,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" t="s">
         <v>71</v>
-      </c>
-      <c r="B33" t="s">
-        <v>72</v>
       </c>
       <c r="C33">
         <v>323877</v>
@@ -1738,10 +1737,10 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" t="s">
         <v>73</v>
-      </c>
-      <c r="B34" t="s">
-        <v>74</v>
       </c>
       <c r="C34">
         <v>301277</v>
@@ -1755,10 +1754,10 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>74</v>
+      </c>
+      <c r="B35" t="s">
         <v>75</v>
-      </c>
-      <c r="B35" t="s">
-        <v>76</v>
       </c>
       <c r="C35">
         <v>92389</v>
@@ -1772,10 +1771,10 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>76</v>
+      </c>
+      <c r="B36" t="s">
         <v>77</v>
-      </c>
-      <c r="B36" t="s">
-        <v>78</v>
       </c>
       <c r="C36">
         <v>237500</v>
@@ -1784,15 +1783,15 @@
         <v>23.2</v>
       </c>
       <c r="E36" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B37" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C37">
         <v>61</v>
@@ -1806,10 +1805,10 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>79</v>
+      </c>
+      <c r="B38" t="s">
         <v>80</v>
-      </c>
-      <c r="B38" t="s">
-        <v>81</v>
       </c>
       <c r="C38">
         <v>504782</v>
@@ -1823,10 +1822,10 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>81</v>
+      </c>
+      <c r="B39" t="s">
         <v>82</v>
-      </c>
-      <c r="B39" t="s">
-        <v>83</v>
       </c>
       <c r="C39">
         <v>41293</v>
@@ -1840,10 +1839,10 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>83</v>
+      </c>
+      <c r="B40" t="s">
         <v>84</v>
-      </c>
-      <c r="B40" t="s">
-        <v>85</v>
       </c>
       <c r="C40">
         <v>449964</v>
@@ -1857,10 +1856,10 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>85</v>
+      </c>
+      <c r="B41" t="s">
         <v>86</v>
-      </c>
-      <c r="B41" t="s">
-        <v>87</v>
       </c>
       <c r="C41">
         <v>66577</v>
@@ -1874,10 +1873,10 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>87</v>
+      </c>
+      <c r="B42" t="s">
         <v>88</v>
-      </c>
-      <c r="B42" t="s">
-        <v>89</v>
       </c>
       <c r="C42">
         <v>49035</v>
@@ -1891,10 +1890,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
+        <v>89</v>
+      </c>
+      <c r="B43" t="s">
         <v>90</v>
-      </c>
-      <c r="B43" t="s">
-        <v>91</v>
       </c>
       <c r="C43">
         <v>20250</v>
@@ -1908,10 +1907,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
+        <v>91</v>
+      </c>
+      <c r="B44" t="s">
         <v>92</v>
-      </c>
-      <c r="B44" t="s">
-        <v>93</v>
       </c>
       <c r="C44">
         <v>603700</v>
@@ -1920,7 +1919,7 @@
         <v>51.8</v>
       </c>
       <c r="E44" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>